<commit_message>
Building the main function
</commit_message>
<xml_diff>
--- a/inst/extdata/Defaults.xlsx
+++ b/inst/extdata/Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Desktop/Git_Repos/ProteoMatch/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B600437-450F-AD40-B885-89EAAD428F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CB233-CCB0-094D-9052-553AE0220BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>ProtonMass</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>An abundance (every peak is scaled to the largest peak) cutoff for peaks. A reasonable value should be in the 2.5 - 5.0% range. Default is 5%.</t>
+  </si>
+  <si>
+    <t>Charges</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>The range of charges to test. List charges separated by a comma</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25419109-B18E-184C-810E-4DA843070287}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,71 +520,85 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>1.0072764700000001</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1.0072764700000001</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding noise filter to matching algorithm
</commit_message>
<xml_diff>
--- a/inst/extdata/Defaults.xlsx
+++ b/inst/extdata/Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Desktop/Git_Repos/ProteoMatch/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CB233-CCB0-094D-9052-553AE0220BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05436B30-FB12-4F47-892A-5E182CFB54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>ProtonMass</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>The range of charges to test. List charges separated by a comma</t>
+  </si>
+  <si>
+    <t>CorrelationMinimum</t>
+  </si>
+  <si>
+    <t>The minimum correlation value to consider when generating the trelliscope display</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25419109-B18E-184C-810E-4DA843070287}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A4:D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,71 +540,85 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>1.0072764700000001</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1.0072764700000001</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Storing current version before intensity value assumptions
</commit_message>
<xml_diff>
--- a/inst/extdata/Defaults.xlsx
+++ b/inst/extdata/Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Desktop/Git_Repos/ProteoMatch/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05436B30-FB12-4F47-892A-5E182CFB54E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8098A7C9-AC00-2A45-927C-3BFE2111BAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>ProtonMass</t>
   </si>
@@ -55,9 +55,6 @@
     <t>PPMThreshold</t>
   </si>
   <si>
-    <t>MaxIsotopes</t>
-  </si>
-  <si>
     <t>PlottingWindow</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>The maximum m/z error permitted. </t>
   </si>
   <si>
-    <t>The maximum number of isotopes to consider</t>
-  </si>
-  <si>
     <t>The -/+ m/z value on either side of the matched spectra plot. Default is 2 m/z.</t>
   </si>
   <si>
@@ -116,6 +110,24 @@
   </si>
   <si>
     <t>The minimum correlation value to consider when generating the trelliscope display</t>
+  </si>
+  <si>
+    <t>IsotopeRange</t>
+  </si>
+  <si>
+    <t>The minimum and maximum number of isotopes to consider</t>
+  </si>
+  <si>
+    <t>Occasionally</t>
+  </si>
+  <si>
+    <t>MinAbsoluteChange</t>
+  </si>
+  <si>
+    <t>An abundance (every peak is scaled to the largest peak) absolute change required to count a subsequent peak as an isotope. Default is 0.5.</t>
+  </si>
+  <si>
+    <t>5,20</t>
   </si>
 </sst>
 </file>
@@ -151,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25419109-B18E-184C-810E-4DA843070287}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -498,128 +511,142 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>1.0072764700000001</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>